<commit_message>
corrigindo parametros e erro de disps infinitos
</commit_message>
<xml_diff>
--- a/planilhas/objetos.xlsx
+++ b/planilhas/objetos.xlsx
@@ -412,33 +412,14 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>ar 1</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>A/C</t>
-        </is>
-      </c>
-      <c r="C1" t="n">
-        <v>23</v>
-      </c>
-      <c r="D1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
corrigindo erro das automações
</commit_message>
<xml_diff>
--- a/planilhas/objetos.xlsx
+++ b/planilhas/objetos.xlsx
@@ -445,10 +445,10 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
@@ -463,13 +463,13 @@
         </is>
       </c>
       <c r="C2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>50</v>
+      </c>
+      <c r="E2" t="b">
         <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>

</xml_diff>